<commit_message>
Màj maquette, use cases et journal
</commit_message>
<xml_diff>
--- a/Documentation/journal_de_travail_AGI.xlsx
+++ b/Documentation/journal_de_travail_AGI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Jeudi 01.02.2018</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Création du repository Github, création de la maquette, création de quelques use case scénarios</t>
+  </si>
+  <si>
+    <t>Ajout de la page commande à la maquette et ajout de use case scénarios</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
mise à jour maquettes et use case
</commit_message>
<xml_diff>
--- a/Documentation/journal_de_travail_AGI.xlsx
+++ b/Documentation/journal_de_travail_AGI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Jeudi 01.02.2018</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Ajout de la page commande à la maquette et ajout de use case scénarios</t>
+  </si>
+  <si>
+    <t>Mise à jour maquette et use case scénarios</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +506,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Modification maquettes, use cases, journal de travail et création dossier projet et MCD
</commit_message>
<xml_diff>
--- a/Documentation/journal_de_travail_AGI.xlsx
+++ b/Documentation/journal_de_travail_AGI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Jeudi 01.02.2018</t>
   </si>
@@ -68,15 +68,6 @@
     <t>Création du planning initial</t>
   </si>
   <si>
-    <t>180 min</t>
-  </si>
-  <si>
-    <t>135 min</t>
-  </si>
-  <si>
-    <t>270 min</t>
-  </si>
-  <si>
     <t>Création du repository Github, création de la maquette, création de quelques use case scénarios</t>
   </si>
   <si>
@@ -84,13 +75,79 @@
   </si>
   <si>
     <t>Mise à jour maquette et use case scénarios</t>
+  </si>
+  <si>
+    <t>Temps (en minutes)</t>
+  </si>
+  <si>
+    <t>Mardi 27.02.2018</t>
+  </si>
+  <si>
+    <t>Mercredi 28.02.2018</t>
+  </si>
+  <si>
+    <t>Jeudi 01.03.2018</t>
+  </si>
+  <si>
+    <t>Vendredi 02.03.2018</t>
+  </si>
+  <si>
+    <t>Mardi 06.03.2018</t>
+  </si>
+  <si>
+    <t>Mercredi 07.03.2018</t>
+  </si>
+  <si>
+    <t>Jeudi 08.03.2018</t>
+  </si>
+  <si>
+    <t>Vendredi 09.03.2018</t>
+  </si>
+  <si>
+    <t>Mardi 13.03.2018</t>
+  </si>
+  <si>
+    <t>Mercredi 14.03.2018</t>
+  </si>
+  <si>
+    <t>Jeudi 15.03.2018</t>
+  </si>
+  <si>
+    <t>Vendredi 16.03.2018</t>
+  </si>
+  <si>
+    <t>Mardi 20.03.2018</t>
+  </si>
+  <si>
+    <t>Mercredi 21.03.2018</t>
+  </si>
+  <si>
+    <t>Jeudi 22.03.2018</t>
+  </si>
+  <si>
+    <t>Vendredi 23.03.2018</t>
+  </si>
+  <si>
+    <t>Tâches</t>
+  </si>
+  <si>
+    <t>Jours</t>
+  </si>
+  <si>
+    <t>Mise au point</t>
+  </si>
+  <si>
+    <t>Temps total (en minutes)</t>
+  </si>
+  <si>
+    <t>Mise à jour maquette, use case scénarios et journal de travail d'après la mise au point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,16 +155,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,15 +186,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,126 +511,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="1" max="1" width="65" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="5">
+        <v>180</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5">
+        <v>135</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>270</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>135</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>180</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>135</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B8" s="5">
+        <v>270</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B9" s="5">
+        <v>135</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B10" s="5">
+        <v>180</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B11" s="5">
+        <v>135</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8">
+        <v>30</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D12" s="10">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8">
+        <v>240</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5">
+        <v>135</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
+      <c r="D14" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5">
+        <v>180</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5">
+        <v>135</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5">
+        <v>270</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5">
+        <v>135</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5">
+        <v>180</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5">
+        <v>135</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5">
+        <v>270</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5">
+        <v>135</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5">
+        <v>180</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5">
+        <v>135</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5">
+        <v>270</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5">
+        <v>135</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5">
+        <v>180</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5">
+        <v>135</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="7">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>